<commit_message>
Adding extra column to excel test data spreadsheet
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
   <si>
     <t>Sample ID</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>abc</t>
+  </si>
+  <si>
+    <t>Sort Column</t>
   </si>
 </sst>
 </file>
@@ -256,7 +259,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,12 +274,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -616,27 +623,28 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="38" customWidth="1"/>
-    <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,24 +672,27 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="8"/>
+      <c r="M1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="8"/>
+      <c r="O1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="7"/>
-      <c r="P1" s="8" t="s">
+      <c r="P1" s="8"/>
+      <c r="Q1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="7"/>
-    </row>
-    <row r="2" spans="1:17">
+      <c r="R1" s="8"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -709,8 +720,9 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -738,32 +750,33 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="1"/>
+      <c r="K3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -788,29 +801,32 @@
       <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K4">
-        <v>0</v>
+      <c r="J4" s="10">
+        <v>1</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
         <v>0</v>
       </c>
       <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
         <v>2</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -835,32 +851,35 @@
       <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J5">
-        <v>0</v>
+      <c r="J5" s="10">
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O5">
         <v>0</v>
       </c>
       <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>2</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -885,32 +904,35 @@
       <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J6">
-        <v>1</v>
+      <c r="J6" s="10">
+        <v>3</v>
       </c>
       <c r="K6">
+        <v>1</v>
+      </c>
+      <c r="L6">
         <v>2</v>
       </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
         <v>0</v>
       </c>
       <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
         <v>2</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -935,37 +957,40 @@
       <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7" s="10">
+        <v>4</v>
+      </c>
+      <c r="K7" t="s">
         <v>37</v>
       </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
       <c r="L7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7">
         <v>0</v>
       </c>
       <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>2</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1033,16 +1058,16 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="7"/>
-      <c r="L1" s="6"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="7"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="7"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="8"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" s="1" t="s">

</xml_diff>

<commit_message>
GPLIM-1: Get test data correct
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1220" yWindow="3120" windowWidth="46660" windowHeight="15760"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="23320"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
     <sheet name="P-EXEX-0001" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
   <si>
     <t>Sample ID</t>
   </si>
@@ -158,12 +158,21 @@
   <si>
     <t>Sort Column</t>
   </si>
+  <si>
+    <t>RNA:Total RNA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -214,6 +223,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -252,14 +267,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -275,26 +292,22 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -619,392 +632,407 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="11.5" style="6" customWidth="1"/>
-    <col min="11" max="11" width="38" customWidth="1"/>
-    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.875" style="9"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="8" customWidth="1"/>
+    <col min="12" max="12" width="38" customWidth="1"/>
+    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="8"/>
-      <c r="M1" s="7" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="8"/>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="8"/>
+      <c r="S1" s="2"/>
     </row>
-    <row r="2" spans="1:18">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1"/>
+    <row r="2" spans="1:19">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="3"/>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1"/>
-      <c r="K3" s="2" t="s">
+    <row r="3" spans="1:19">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="L3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="2" t="s">
+      <c r="P3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>21</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="10">
+      <c r="J4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="10">
         <v>1</v>
       </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
       <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
         <v>1</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>21</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>22</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="10">
+      <c r="J5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="10">
         <v>2</v>
       </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
       <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>1</v>
       </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
       <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
         <v>1</v>
       </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
       <c r="P5">
         <v>0</v>
       </c>
       <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
         <v>2</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>0.5</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="10">
+      <c r="J6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="10">
         <v>3</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <v>2</v>
       </c>
-      <c r="M6">
-        <v>0</v>
-      </c>
       <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>1</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
         <v>2</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:19">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7" s="10">
+      <c r="J7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="10">
         <v>4</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>37</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <v>1</v>
       </c>
-      <c r="M7">
-        <v>0</v>
-      </c>
       <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
         <v>1</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
       <c r="P7">
         <v>0</v>
       </c>
       <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
         <v>2</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" fitToWidth="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1014,130 +1042,130 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="46.125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" customWidth="1"/>
     <col min="10" max="10" width="38" customWidth="1"/>
     <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="7"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="8"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="A3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="K3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
+      <c r="L3" s="4"/>
+      <c r="M3" s="4"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
+      <c r="Q3" s="4"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -1161,7 +1189,7 @@
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J4">
@@ -1178,7 +1206,7 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
@@ -1193,7 +1221,7 @@
       <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I5" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J5">
@@ -1210,7 +1238,7 @@
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D6" t="s">
@@ -1225,7 +1253,7 @@
       <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J6">
@@ -1242,7 +1270,7 @@
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D7" t="s">
@@ -1257,7 +1285,7 @@
       <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="J7">
@@ -1276,10 +1304,9 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="60" fitToWidth="2" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>

<commit_message>
GPLIM-1: Get test data correct for real (forgot to add the header to this file)
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="34400" windowHeight="23320"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="26040" windowHeight="12560"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="41">
   <si>
     <t>Sample ID</t>
   </si>
@@ -160,6 +160,10 @@
   </si>
   <si>
     <t>RNA:Total RNA</t>
+  </si>
+  <si>
+    <t>Material Type</t>
+    <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -274,10 +278,6 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -296,10 +296,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -639,15 +643,15 @@
   <dimension ref="A1:S7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="9"/>
+    <col min="3" max="3" width="8.875" style="7"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="8" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="6" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
     <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
@@ -659,137 +663,139 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="1" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="11"/>
+      <c r="P1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="11" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="2"/>
+      <c r="S1" s="11"/>
     </row>
     <row r="2" spans="1:19">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="3"/>
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="L3" s="4" t="s">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M3" s="4" t="s">
+      <c r="M3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O3" s="4" t="s">
+      <c r="O3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P3" s="4" t="s">
+      <c r="P3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="4" t="s">
+      <c r="Q3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R3" s="4" t="s">
+      <c r="R3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S3" s="4" t="s">
+      <c r="S3" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -800,7 +806,7 @@
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
@@ -818,10 +824,10 @@
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="10">
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4" s="8">
         <v>1</v>
       </c>
       <c r="M4">
@@ -853,7 +859,7 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
@@ -871,10 +877,10 @@
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="10">
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="8">
         <v>2</v>
       </c>
       <c r="L5">
@@ -909,7 +915,7 @@
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D6" t="s">
@@ -927,10 +933,10 @@
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="10">
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="8">
         <v>3</v>
       </c>
       <c r="L6">
@@ -965,7 +971,7 @@
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D7" t="s">
@@ -983,10 +989,10 @@
       <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="10">
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="8">
         <v>4</v>
       </c>
       <c r="L7" t="s">
@@ -1015,6 +1021,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
@@ -1059,113 +1066,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="2"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="11"/>
     </row>
     <row r="2" spans="1:17">
-      <c r="A2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="3" t="s">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="7" t="s">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
     <row r="4" spans="1:17">
       <c r="A4" t="s">
@@ -1189,7 +1196,7 @@
       <c r="H4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J4">
@@ -1206,7 +1213,7 @@
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D5" t="s">
@@ -1221,7 +1228,7 @@
       <c r="H5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J5">
@@ -1238,7 +1245,7 @@
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D6" t="s">
@@ -1253,7 +1260,7 @@
       <c r="H6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J6">
@@ -1270,7 +1277,7 @@
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4" t="s">
         <v>36</v>
       </c>
       <c r="D7" t="s">
@@ -1285,7 +1292,7 @@
       <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="J7">
@@ -1296,6 +1303,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>

</xml_diff>

<commit_message>
GPLIM-1: Add dates AND fixed header of second worksheet
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="26040" windowHeight="12560"/>
+    <workbookView xWindow="4160" yWindow="6900" windowWidth="26040" windowHeight="12560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
   <si>
     <t>Sample ID</t>
   </si>
@@ -276,7 +276,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -297,6 +297,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -304,6 +305,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -642,14 +644,17 @@
   </sheetPr>
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.875" style="7"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="6" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
@@ -696,22 +701,22 @@
       <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="L1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="10" t="s">
+      <c r="M1" s="12"/>
+      <c r="N1" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="11"/>
-      <c r="P1" s="12" t="s">
+      <c r="O1" s="12"/>
+      <c r="P1" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="12" t="s">
+      <c r="Q1" s="12"/>
+      <c r="R1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="11"/>
+      <c r="S1" s="12"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
@@ -821,6 +826,9 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
+      <c r="H4" s="14">
+        <v>41239</v>
+      </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
@@ -874,6 +882,9 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
+      <c r="H5" s="14">
+        <v>41239</v>
+      </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
@@ -930,6 +941,9 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
+      <c r="H6" s="14">
+        <v>41239</v>
+      </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
@@ -985,6 +999,9 @@
       </c>
       <c r="G7" t="s">
         <v>23</v>
+      </c>
+      <c r="H7" s="14">
+        <v>41239</v>
       </c>
       <c r="I7" t="s">
         <v>24</v>
@@ -1030,6 +1047,7 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1043,29 +1061,30 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:R7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="46.125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5" customWidth="1"/>
-    <col min="10" max="10" width="38" customWidth="1"/>
-    <col min="11" max="11" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="10" customWidth="1"/>
+    <col min="4" max="4" width="46.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1073,47 +1092,48 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="10" t="s">
+      <c r="K1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="11"/>
-      <c r="L1" s="10"/>
+      <c r="L1" s="12"/>
       <c r="M1" s="11"/>
       <c r="N1" s="12"/>
-      <c r="O1" s="11"/>
+      <c r="O1" s="13"/>
       <c r="P1" s="12"/>
-      <c r="Q1" s="11"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="12"/>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:18">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1132,17 +1152,18 @@
       <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
         <v>13</v>
       </c>
@@ -1161,154 +1182,169 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="L3" s="2"/>
       <c r="M3" s="2"/>
       <c r="N3" s="2"/>
       <c r="O3" s="2"/>
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>34</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="I4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4">
+      <c r="J4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K4">
         <v>1</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5">
+      <c r="J5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5">
         <v>1</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>27</v>
       </c>
       <c r="B6" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>33</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>34</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="I6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6">
+      <c r="J6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6">
         <v>1</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>34</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>24</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="J7">
+      <c r="J7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7">
         <v>1</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
GPLIM_373_BillingTracker_Persist - Billing tracker persistence.
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="6900" windowWidth="26040" windowHeight="12560" activeTab="1"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
   <si>
     <t>Sample ID</t>
   </si>
@@ -169,14 +169,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -271,12 +265,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -298,6 +300,8 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -305,15 +309,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
@@ -638,33 +649,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="11.5" style="6" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
     <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -701,22 +712,22 @@
       <c r="K1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="L1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="12"/>
-      <c r="N1" s="11" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="13" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="13" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="12"/>
+      <c r="S1" s="14"/>
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
@@ -748,68 +759,93 @@
         <v>13</v>
       </c>
       <c r="K2" s="1"/>
+      <c r="L2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="1"/>
-      <c r="L3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="R3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>17</v>
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="12">
+        <v>41239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>0.5</v>
       </c>
     </row>
     <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>39</v>
@@ -826,7 +862,7 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="12">
         <v>41239</v>
       </c>
       <c r="I4" t="s">
@@ -836,10 +872,13 @@
         <v>13</v>
       </c>
       <c r="K4" s="8">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
       </c>
       <c r="M4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -862,10 +901,10 @@
     </row>
     <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>39</v>
@@ -882,7 +921,7 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="12">
         <v>41239</v>
       </c>
       <c r="I5" t="s">
@@ -892,13 +931,13 @@
         <v>13</v>
       </c>
       <c r="K5" s="8">
+        <v>3</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>2</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -921,10 +960,10 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>39</v>
@@ -941,7 +980,7 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="14">
+      <c r="H6" s="12">
         <v>41239</v>
       </c>
       <c r="I6" t="s">
@@ -951,13 +990,13 @@
         <v>13</v>
       </c>
       <c r="K6" s="8">
-        <v>3</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
       </c>
       <c r="M6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -978,67 +1017,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="7" spans="1:19">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="14">
-        <v>41239</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7" s="8">
-        <v>4</v>
-      </c>
-      <c r="L7" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7">
-        <v>1</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>1</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-      <c r="R7">
-        <v>2</v>
-      </c>
-      <c r="S7">
-        <v>0.5</v>
-      </c>
-    </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
@@ -1049,7 +1028,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1057,34 +1036,37 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R7"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.875" customWidth="1"/>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="10" customWidth="1"/>
-    <col min="4" max="4" width="46.125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="38" customWidth="1"/>
-    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.83203125" style="11"/>
+    <col min="11" max="11" width="11.5" customWidth="1"/>
+    <col min="12" max="12" width="38" customWidth="1"/>
+    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1115,18 +1097,21 @@
       <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="K1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="12"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="12"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="14"/>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:19">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1155,60 +1140,74 @@
       <c r="J2" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="2"/>
+      <c r="R2" s="2"/>
+      <c r="S2" s="2"/>
     </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+    <row r="3" spans="1:19">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="12">
+        <v>41239</v>
+      </c>
+      <c r="I3" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>8</v>
+      </c>
     </row>
-    <row r="4" spans="1:18">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E4" t="s">
@@ -1220,25 +1219,31 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
+      <c r="H4" s="12">
+        <v>41239</v>
+      </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K4">
-        <v>1</v>
+      <c r="K4" s="8">
+        <v>2</v>
       </c>
       <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>39</v>
@@ -1255,25 +1260,31 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
+      <c r="H5" s="12">
+        <v>41239</v>
+      </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K5">
-        <v>1</v>
+      <c r="K5" s="8">
+        <v>3</v>
       </c>
       <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>39</v>
@@ -1290,66 +1301,37 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
+      <c r="H6" s="12">
+        <v>41239</v>
+      </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="K6">
-        <v>1</v>
+      <c r="K6" s="8">
+        <v>4</v>
       </c>
       <c r="L6">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M6">
         <v>8</v>
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
GPLIM-1: Fixed date, column sizes, where errors show up, test data, some styling
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22221"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560" activeTab="1"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -169,8 +169,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -265,21 +271,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -302,29 +307,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -649,149 +639,149 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="6" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" style="9" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
     <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="54.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:20">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="2"/>
+      <c r="P1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S1" s="2"/>
+      <c r="T1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="S1" s="14"/>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="2" t="s">
+    <row r="2" spans="1:20">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="N2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="O2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="P2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="Q2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="R2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="T2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D3" t="s">
@@ -806,16 +796,13 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="15">
         <v>41239</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="K3" s="11">
         <v>1</v>
       </c>
       <c r="M3">
@@ -839,15 +826,18 @@
       <c r="S3">
         <v>0.5</v>
       </c>
+      <c r="T3" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
@@ -862,16 +852,13 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="15">
         <v>41239</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="8">
+      <c r="K4" s="11">
         <v>2</v>
       </c>
       <c r="L4">
@@ -898,15 +885,18 @@
       <c r="S4">
         <v>0.5</v>
       </c>
+      <c r="T4" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
@@ -921,16 +911,13 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="15">
         <v>41239</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="8">
+      <c r="K5" s="11">
         <v>3</v>
       </c>
       <c r="L5">
@@ -957,15 +944,18 @@
       <c r="S5">
         <v>0.5</v>
       </c>
+      <c r="T5" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D6" t="s">
@@ -980,16 +970,13 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="15">
         <v>41239</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="K6" s="11">
         <v>4</v>
       </c>
       <c r="L6" t="s">
@@ -1015,6 +1002,9 @@
       </c>
       <c r="S6">
         <v>0.5</v>
+      </c>
+      <c r="T6" s="6" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -1028,7 +1018,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
@@ -1036,134 +1026,116 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="46.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.83203125" style="11"/>
+    <col min="1" max="1" width="13.875" customWidth="1"/>
+    <col min="2" max="2" width="17.125" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="13" customWidth="1"/>
+    <col min="4" max="4" width="46.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" customWidth="1"/>
     <col min="12" max="12" width="38" customWidth="1"/>
-    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="M1" s="2"/>
+      <c r="N1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="14"/>
     </row>
-    <row r="2" spans="1:19">
-      <c r="A2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="5" t="s">
+    <row r="2" spans="1:14">
+      <c r="A2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
+      <c r="N2" s="4" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D3" t="s">
@@ -1178,16 +1150,13 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="12">
+      <c r="H3" s="15">
         <v>41239</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" s="8">
+      <c r="K3" s="11">
         <v>1</v>
       </c>
       <c r="L3">
@@ -1196,18 +1165,21 @@
       <c r="M3">
         <v>8</v>
       </c>
+      <c r="N3" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E4" t="s">
@@ -1219,16 +1191,13 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="15">
         <v>41239</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="J4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K4" s="8">
+      <c r="K4" s="11">
         <v>2</v>
       </c>
       <c r="L4">
@@ -1237,18 +1206,21 @@
       <c r="M4">
         <v>8</v>
       </c>
+      <c r="N4" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E5" t="s">
@@ -1260,16 +1232,13 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="12">
+      <c r="H5" s="15">
         <v>41239</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K5" s="8">
+      <c r="K5" s="11">
         <v>3</v>
       </c>
       <c r="L5">
@@ -1278,18 +1247,21 @@
       <c r="M5">
         <v>8</v>
       </c>
+      <c r="N5" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="7" t="s">
         <v>36</v>
       </c>
       <c r="E6" t="s">
@@ -1301,16 +1273,13 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="12">
+      <c r="H6" s="15">
         <v>41239</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="J6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K6" s="8">
+      <c r="K6" s="11">
         <v>4</v>
       </c>
       <c r="L6">
@@ -1319,19 +1288,19 @@
       <c r="M6">
         <v>8</v>
       </c>
+      <c r="N6" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="1">
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
GPLIM-1: Remove empty column that was supposed to be moved
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -278,13 +278,6 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -307,6 +300,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -643,145 +643,145 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:T6"/>
+  <dimension ref="A1:S6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1:T1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="7" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" style="9" customWidth="1"/>
-    <col min="12" max="12" width="38" customWidth="1"/>
-    <col min="13" max="13" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="54.125" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="6" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="31.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="32.375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="54.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:19">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="3" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="1" t="s">
+      <c r="N1" s="14"/>
+      <c r="O1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="1" t="s">
+      <c r="P1" s="14"/>
+      <c r="Q1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="4" t="s">
+      <c r="R1" s="14"/>
+      <c r="S1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:20">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="4"/>
-      <c r="L2" s="5" t="s">
+    <row r="2" spans="1:19">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1"/>
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="L2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="N2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="P2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="Q2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="S2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:20">
+    <row r="3" spans="1:19">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D3" t="s">
@@ -796,48 +796,48 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="12">
         <v>41239</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="11">
-        <v>1</v>
+      <c r="J3" s="8">
+        <v>1</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
       </c>
       <c r="M3">
         <v>0</v>
       </c>
       <c r="N3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R3">
-        <v>2</v>
-      </c>
-      <c r="S3">
         <v>0.5</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="S3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:20">
+    <row r="4" spans="1:19">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D4" t="s">
@@ -852,51 +852,51 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="12">
         <v>41239</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="11">
+      <c r="J4" s="8">
         <v>2</v>
       </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
       <c r="L4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R4">
-        <v>2</v>
-      </c>
-      <c r="S4">
         <v>0.5</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="S4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:20">
+    <row r="5" spans="1:19">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D5" t="s">
@@ -911,51 +911,51 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="12">
         <v>41239</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="11">
+      <c r="J5" s="8">
         <v>3</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
       <c r="L5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
         <v>2</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
       <c r="R5">
-        <v>2</v>
-      </c>
-      <c r="S5">
         <v>0.5</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="S5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:20">
+    <row r="6" spans="1:19">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D6" t="s">
@@ -970,53 +970,52 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="12">
         <v>41239</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="11">
+      <c r="J6" s="8">
         <v>4</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s">
         <v>37</v>
       </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
       <c r="M6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6">
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="R6">
-        <v>2</v>
-      </c>
-      <c r="S6">
         <v>0.5</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="S6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="L1:M1"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1030,112 +1029,112 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1:N1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.875" customWidth="1"/>
     <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="3" max="3" width="10.875" style="13" customWidth="1"/>
+    <col min="3" max="3" width="10.875" style="10" customWidth="1"/>
     <col min="4" max="4" width="46.125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5" customWidth="1"/>
-    <col min="12" max="12" width="38" customWidth="1"/>
-    <col min="13" max="13" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.875" style="14"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
+    <col min="11" max="11" width="38" customWidth="1"/>
+    <col min="12" max="12" width="20.875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
+    <row r="1" spans="1:13">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="K1" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="4" t="s">
+      <c r="L1" s="14"/>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="8" t="s">
+    <row r="2" spans="1:13">
+      <c r="A2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="M2" s="8" t="s">
+      <c r="L2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="N2" s="4" t="s">
+      <c r="M2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:14">
+    <row r="3" spans="1:13">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="9" t="s">
         <v>39</v>
       </c>
       <c r="D3" t="s">
@@ -1150,36 +1149,36 @@
       <c r="G3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H3" s="12">
         <v>41239</v>
       </c>
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="11">
+      <c r="J3" s="8">
+        <v>1</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
       <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
         <v>8</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="M3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:13">
       <c r="A4" t="s">
         <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E4" t="s">
@@ -1191,36 +1190,36 @@
       <c r="G4" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="12">
         <v>41239</v>
       </c>
       <c r="I4" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="11">
+      <c r="J4" s="8">
         <v>2</v>
       </c>
+      <c r="K4">
+        <v>1</v>
+      </c>
       <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
         <v>8</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:13">
       <c r="A5" t="s">
         <v>27</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E5" t="s">
@@ -1232,36 +1231,36 @@
       <c r="G5" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="12">
         <v>41239</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="11">
+      <c r="J5" s="8">
         <v>3</v>
       </c>
+      <c r="K5">
+        <v>1</v>
+      </c>
       <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
         <v>8</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="M5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:13">
       <c r="A6" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="E6" t="s">
@@ -1273,32 +1272,31 @@
       <c r="G6" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="12">
         <v>41239</v>
       </c>
       <c r="I6" t="s">
         <v>24</v>
       </c>
-      <c r="K6" s="11">
+      <c r="J6" s="8">
         <v>4</v>
       </c>
+      <c r="K6">
+        <v>1</v>
+      </c>
       <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
         <v>8</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="M6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
GPLIM-474: Add product order comments to comment field
</commit_message>
<xml_diff>
--- a/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
+++ b/mercury/src/test/data/billing/BillingTracker-DBFreeTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560" activeTab="1"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="26040" windowHeight="12560"/>
   </bookViews>
   <sheets>
     <sheet name="P-RNA-0004" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>Sample ID</t>
   </si>
@@ -165,17 +165,19 @@
     <t>Material Type</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
+  <si>
+    <t>Comments</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>Comments</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="9">
     <font>
       <sz val="11"/>
@@ -276,7 +278,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -300,6 +302,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -643,10 +646,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:T6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -665,10 +668,11 @@
     <col min="16" max="16" width="36.625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="32.375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="36.625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="54.125" customWidth="1"/>
+    <col min="19" max="19" width="36.625" style="13" customWidth="1"/>
+    <col min="20" max="20" width="54.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
+    <row r="1" spans="1:20">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,27 +703,30 @@
       <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="14"/>
-      <c r="M1" s="13" t="s">
+      <c r="L1" s="15"/>
+      <c r="M1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="14"/>
-      <c r="O1" s="15" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="15" t="s">
+      <c r="P1" s="15"/>
+      <c r="Q1" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="14"/>
-      <c r="S1" s="1" t="s">
+      <c r="R1" s="15"/>
+      <c r="S1" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:19">
+    <row r="2" spans="1:20">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -770,11 +777,12 @@
       <c r="R2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="S2" s="2"/>
+      <c r="T2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -826,11 +834,11 @@
       <c r="R3">
         <v>0.5</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="T3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -885,11 +893,11 @@
       <c r="R4">
         <v>0.5</v>
       </c>
-      <c r="S4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:19">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -944,11 +952,11 @@
       <c r="R5">
         <v>0.5</v>
       </c>
-      <c r="S5" s="3" t="s">
+      <c r="T5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:19">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1003,7 +1011,7 @@
       <c r="R6">
         <v>0.5</v>
       </c>
-      <c r="S6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1029,10 +1037,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.875" defaultRowHeight="15"/>
@@ -1046,10 +1054,11 @@
     <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="38" customWidth="1"/>
     <col min="12" max="12" width="20.875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.875" style="11"/>
+    <col min="13" max="13" width="20.875" style="13" customWidth="1"/>
+    <col min="14" max="14" width="8.875" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1080,15 +1089,18 @@
       <c r="J1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="K1" s="13" t="s">
+      <c r="K1" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="L1" s="14"/>
+      <c r="L1" s="15"/>
       <c r="M1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:14">
       <c r="A2" s="1" t="s">
         <v>13</v>
       </c>
@@ -1123,11 +1135,12 @@
       <c r="L2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="5"/>
+      <c r="N2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1164,11 +1177,11 @@
       <c r="L3">
         <v>8</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="N3" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1205,11 +1218,11 @@
       <c r="L4">
         <v>8</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1246,11 +1259,11 @@
       <c r="L5">
         <v>8</v>
       </c>
-      <c r="M5" s="3" t="s">
+      <c r="N5" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>29</v>
       </c>
@@ -1287,7 +1300,7 @@
       <c r="L6">
         <v>8</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>